<commit_message>
Added Pert Values to user_stories.xlsx and PERT diagram to PP directory.
</commit_message>
<xml_diff>
--- a/Evidence/PP/user_stories.xlsx
+++ b/Evidence/PP/user_stories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raygu\Downloads\CO3095-Group-16-Music-Player-Application\User Stories\Planning Poker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raygu\Downloads\CO3095-Group-16-Music-Player-Application\Evidence\PP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4221FB-5F3D-44D2-BF04-BCDCFA2AE40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61672AE3-06B7-442D-9F0C-D83468A63926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
   <si>
     <t>User Story</t>
   </si>
@@ -210,13 +210,64 @@
   </si>
   <si>
     <t>Expected (Hours)</t>
+  </si>
+  <si>
+    <t>Predecessor</t>
+  </si>
+  <si>
+    <t>S1-01</t>
+  </si>
+  <si>
+    <t>S1-02</t>
+  </si>
+  <si>
+    <t>S1-12</t>
+  </si>
+  <si>
+    <t>S1-03</t>
+  </si>
+  <si>
+    <t>S1-04</t>
+  </si>
+  <si>
+    <t>S1-05</t>
+  </si>
+  <si>
+    <t>S1-06</t>
+  </si>
+  <si>
+    <t>S1-07</t>
+  </si>
+  <si>
+    <t>S1-08</t>
+  </si>
+  <si>
+    <t>S1-09</t>
+  </si>
+  <si>
+    <t>S1-10</t>
+  </si>
+  <si>
+    <t>S1-11</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Story ID (PERT)</t>
+  </si>
+  <si>
+    <t>S1-09, 02, 06, 08</t>
+  </si>
+  <si>
+    <t>S1-07, 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +307,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -602,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,9 +675,11 @@
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -648,8 +707,14 @@
       <c r="I1" s="9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -677,8 +742,14 @@
         <f>((F2+(4*G2)+H2)/6)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -706,8 +777,14 @@
         <f t="shared" ref="I3:I49" si="2">((F3+(4*G3)+H3)/6)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -735,8 +812,14 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -764,8 +847,14 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -793,8 +882,14 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -826,8 +921,14 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -855,8 +956,14 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -884,8 +991,14 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -910,11 +1023,17 @@
         <v>1.5</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <f>((F10+(4*G10)+H10)/6)</f>
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -942,8 +1061,14 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -971,8 +1096,14 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1000,8 +1131,14 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1030,7 +1167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1059,7 +1196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -2087,6 +2224,7 @@
       <c r="A53" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>